<commit_message>
Test Execution Log for TAS build 10
</commit_message>
<xml_diff>
--- a/Test/Build 10/TAS_Core_TEL_TAS.02.00.3_20190425_171947.xlsx
+++ b/Test/Build 10/TAS_Core_TEL_TAS.02.00.3_20190425_171947.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaisathompv\Documents\tascore build 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VHAISPFOWLDD\repos\mccf_tascore_documents\Test\TAS_02.00.3.20190425.171947\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607E1D32-EDFD-4FEA-82E9-490363E122C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF71CA86-6C3F-48EA-8069-98428C3501CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="340" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12220" tabRatio="340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1496,20 +1496,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
     </row>
-    <row r="3" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>107</v>
       </c>
@@ -1533,43 +1533,43 @@
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
         <v>149</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31" t="s">
         <v>150</v>
       </c>
@@ -1593,22 +1593,22 @@
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
     </row>
   </sheetData>
@@ -1635,17 +1635,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="18.453125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -1653,7 +1653,7 @@
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22">
         <v>43584</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>43581</v>
       </c>
@@ -1714,26 +1714,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C247" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D254" sqref="D254"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="79.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="19" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>17</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>17</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>18</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>18</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
         <v>21</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
         <v>22</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>23</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>23</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>23</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>23</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
         <v>24</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>24</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>24</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
         <v>24</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
         <v>24</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
         <v>25</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
         <v>25</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
         <v>26</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
         <v>27</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
         <v>27</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
         <v>28</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="20" t="s">
         <v>28</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
         <v>29</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
         <v>29</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
         <v>30</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
         <v>30</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
         <v>31</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="20" t="s">
         <v>31</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
         <v>32</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
         <v>32</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="20" t="s">
         <v>33</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="20" t="s">
         <v>33</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
         <v>34</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="20" t="s">
         <v>34</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="20" t="s">
         <v>35</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="20" t="s">
         <v>35</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="20" t="s">
         <v>36</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="20" t="s">
         <v>36</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="20" t="s">
         <v>37</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="20" t="s">
         <v>37</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="20" t="s">
         <v>38</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="20" t="s">
         <v>38</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="20" t="s">
         <v>39</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="20" t="s">
         <v>39</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="20" t="s">
         <v>40</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="20" t="s">
         <v>40</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="20" t="s">
         <v>41</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="20" t="s">
         <v>41</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="20" t="s">
         <v>42</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="20" t="s">
         <v>42</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="20" t="s">
         <v>43</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="20" t="s">
         <v>43</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="20" t="s">
         <v>44</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="20" t="s">
         <v>44</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="20" t="s">
         <v>45</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="20" t="s">
         <v>45</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="20" t="s">
         <v>46</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="20" t="s">
         <v>46</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="20" t="s">
         <v>47</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="20" t="s">
         <v>47</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="20" t="s">
         <v>48</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="s">
         <v>48</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="20" t="s">
         <v>49</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="20" t="s">
         <v>49</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="20" t="s">
         <v>50</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="20" t="s">
         <v>50</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="20" t="s">
         <v>51</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="s">
         <v>51</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="20" t="s">
         <v>52</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="20" t="s">
         <v>52</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="20" t="s">
         <v>53</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="20" t="s">
         <v>53</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="20" t="s">
         <v>53</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="20" t="s">
         <v>53</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="20" t="s">
         <v>54</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="20" t="s">
         <v>54</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="20" t="s">
         <v>54</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="20" t="s">
         <v>54</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="20" t="s">
         <v>55</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="20" t="s">
         <v>55</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="20" t="s">
         <v>55</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="20" t="s">
         <v>55</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="20" t="s">
         <v>56</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="20" t="s">
         <v>56</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="20" t="s">
         <v>56</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="20" t="s">
         <v>56</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="20" t="s">
         <v>57</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="20" t="s">
         <v>57</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="20" t="s">
         <v>57</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="20" t="s">
         <v>57</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="20" t="s">
         <v>58</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="20" t="s">
         <v>58</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="20" t="s">
         <v>59</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="s">
         <v>59</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="20" t="s">
         <v>60</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="s">
         <v>60</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="s">
         <v>61</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="s">
         <v>61</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="s">
         <v>62</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="20" t="s">
         <v>62</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="20" t="s">
         <v>62</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="s">
         <v>62</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="20" t="s">
         <v>63</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="s">
         <v>63</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="20" t="s">
         <v>63</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="20" t="s">
         <v>63</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="20" t="s">
         <v>64</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="s">
         <v>64</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="20" t="s">
         <v>64</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="20" t="s">
         <v>64</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="20" t="s">
         <v>65</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" s="20" t="s">
         <v>65</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="20" t="s">
         <v>65</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="20" t="s">
         <v>65</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="20" t="s">
         <v>66</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="20" t="s">
         <v>66</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="20" t="s">
         <v>66</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="20" t="s">
         <v>66</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="20" t="s">
         <v>67</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="20" t="s">
         <v>67</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="20" t="s">
         <v>67</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="20" t="s">
         <v>67</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="20" t="s">
         <v>68</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="20" t="s">
         <v>68</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A137" s="20" t="s">
         <v>68</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="20" t="s">
         <v>68</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="20" t="s">
         <v>69</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" s="20" t="s">
         <v>69</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="20" t="s">
         <v>70</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" s="20" t="s">
         <v>70</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="20" t="s">
         <v>71</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="20" t="s">
         <v>71</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="20" t="s">
         <v>72</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="20" t="s">
         <v>72</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" s="20" t="s">
         <v>73</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="20" t="s">
         <v>73</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="20" t="s">
         <v>74</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" s="20" t="s">
         <v>74</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="20" t="s">
         <v>75</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" s="20" t="s">
         <v>75</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="20" t="s">
         <v>76</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" s="20" t="s">
         <v>76</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" s="20" t="s">
         <v>77</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" s="20" t="s">
         <v>77</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="20" t="s">
         <v>78</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A158" s="20" t="s">
         <v>78</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" s="20" t="s">
         <v>79</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" s="20" t="s">
         <v>79</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" s="20" t="s">
         <v>80</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" s="20" t="s">
         <v>80</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="20" t="s">
         <v>81</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="20" t="s">
         <v>81</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" s="20" t="s">
         <v>82</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" s="20" t="s">
         <v>82</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A167" s="20" t="s">
         <v>83</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A168" s="20" t="s">
         <v>83</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" s="20" t="s">
         <v>84</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" s="20" t="s">
         <v>84</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" s="20" t="s">
         <v>85</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" s="20" t="s">
         <v>85</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="20" t="s">
         <v>86</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="20" t="s">
         <v>86</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" s="20" t="s">
         <v>87</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" s="20" t="s">
         <v>87</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" s="20" t="s">
         <v>87</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" s="20" t="s">
         <v>87</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="20" t="s">
         <v>88</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="20" t="s">
         <v>88</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="20" t="s">
         <v>89</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="20" t="s">
         <v>89</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="20" t="s">
         <v>90</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A184" s="20" t="s">
         <v>90</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" s="20" t="s">
         <v>91</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" s="20" t="s">
         <v>91</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="20" t="s">
         <v>92</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A188" s="20" t="s">
         <v>92</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" s="20" t="s">
         <v>93</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190" s="20" t="s">
         <v>93</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" s="20" t="s">
         <v>94</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" s="20" t="s">
         <v>94</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="20" t="s">
         <v>95</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" s="20" t="s">
         <v>95</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A195" s="20" t="s">
         <v>96</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A196" s="20" t="s">
         <v>96</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A197" s="20" t="s">
         <v>97</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A198" s="20" t="s">
         <v>97</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A199" s="20" t="s">
         <v>98</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A200" s="20" t="s">
         <v>98</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A201" s="20" t="s">
         <v>146</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A202" s="20" t="s">
         <v>146</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A203" s="20" t="s">
         <v>99</v>
       </c>
@@ -6405,7 +6405,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A204" s="20" t="s">
         <v>99</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A205" s="20" t="s">
         <v>100</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A206" s="20" t="s">
         <v>100</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A207" s="20" t="s">
         <v>101</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A208" s="20" t="s">
         <v>101</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A209" s="20" t="s">
         <v>102</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A210" s="20" t="s">
         <v>102</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A211" s="20" t="s">
         <v>103</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A212" s="20" t="s">
         <v>103</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A213" s="20" t="s">
         <v>104</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A214" s="20" t="s">
         <v>104</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A215" s="20" t="s">
         <v>105</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A216" s="20" t="s">
         <v>105</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A217" s="20" t="s">
         <v>112</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A218" s="20" t="s">
         <v>112</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A219" s="20" t="s">
         <v>111</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A220" s="20" t="s">
         <v>111</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A221" s="20" t="s">
         <v>110</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A222" s="20" t="s">
         <v>110</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A223" s="20" t="s">
         <v>109</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A224" s="20" t="s">
         <v>109</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225" s="20" t="s">
         <v>108</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A226" s="20" t="s">
         <v>108</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A227" s="20" t="s">
         <v>137</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A228" s="20" t="s">
         <v>137</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A229" s="20" t="s">
         <v>136</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230" s="20" t="s">
         <v>136</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A231" s="20" t="s">
         <v>135</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A232" s="20" t="s">
         <v>135</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A233" s="20" t="s">
         <v>134</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A234" s="20" t="s">
         <v>134</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A235" s="20" t="s">
         <v>133</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A236" s="20" t="s">
         <v>133</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A237" s="20" t="s">
         <v>132</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A238" s="20" t="s">
         <v>132</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A239" s="20" t="s">
         <v>131</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A240" s="20" t="s">
         <v>131</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A241" s="20" t="s">
         <v>130</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A242" s="20" t="s">
         <v>130</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A243" s="20" t="s">
         <v>129</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A244" s="20" t="s">
         <v>129</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A245" s="20" t="s">
         <v>128</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A246" s="20" t="s">
         <v>128</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A247" s="20" t="s">
         <v>127</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A248" s="20" t="s">
         <v>127</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A249" s="20" t="s">
         <v>126</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A250" s="20" t="s">
         <v>126</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A251" s="20" t="s">
         <v>125</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A252" s="20" t="s">
         <v>125</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A253" s="20" t="s">
         <v>124</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A254" s="20" t="s">
         <v>124</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A255" s="20" t="s">
         <v>123</v>
       </c>
@@ -7601,7 +7601,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A256" s="20" t="s">
         <v>123</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A257" s="20" t="s">
         <v>122</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A258" s="20" t="s">
         <v>122</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A259" s="20" t="s">
         <v>121</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A260" s="20" t="s">
         <v>121</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A261" s="20" t="s">
         <v>120</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A262" s="20" t="s">
         <v>120</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A263" s="20" t="s">
         <v>119</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A264" s="20" t="s">
         <v>119</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A265" s="20" t="s">
         <v>118</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A266" s="20" t="s">
         <v>118</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A267" s="20" t="s">
         <v>117</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A268" s="20" t="s">
         <v>117</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A269" s="20" t="s">
         <v>116</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A270" s="20" t="s">
         <v>116</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A271" s="20" t="s">
         <v>115</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A272" s="20" t="s">
         <v>115</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A273" s="20" t="s">
         <v>114</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A274" s="20" t="s">
         <v>114</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A275" s="20" t="s">
         <v>113</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A276" s="20" t="s">
         <v>113</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A277" s="20" t="s">
         <v>113</v>
       </c>

</xml_diff>